<commit_message>
add lat and long coords
</commit_message>
<xml_diff>
--- a/data/bikeshops.xlsx
+++ b/data/bikeshops.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>Pittsburgh</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>bikeshop.state</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
@@ -674,10 +680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,7 +697,7 @@
     <col min="11" max="11" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -703,8 +710,14 @@
       <c r="D1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -717,8 +730,14 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>40.440624999999997</v>
+      </c>
+      <c r="F2">
+        <v>-79.995885999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -731,8 +750,14 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>42.443961000000002</v>
+      </c>
+      <c r="F3">
+        <v>-76.501880999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -745,8 +770,14 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>39.961176000000002</v>
+      </c>
+      <c r="F4">
+        <v>-82.998794000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -759,8 +790,14 @@
       <c r="D5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>42.331426999999998</v>
+      </c>
+      <c r="F5">
+        <v>-83.045754000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -773,8 +810,14 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>39.103118000000002</v>
+      </c>
+      <c r="F6">
+        <v>-84.512020000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -787,8 +830,14 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>38.252665</v>
+      </c>
+      <c r="F7">
+        <v>-85.758455999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -801,8 +850,14 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>36.162663999999999</v>
+      </c>
+      <c r="F8">
+        <v>-86.781602000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -815,8 +870,14 @@
       <c r="D9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>39.739235999999998</v>
+      </c>
+      <c r="F9">
+        <v>-104.990251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -829,8 +890,14 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>44.977753</v>
+      </c>
+      <c r="F10">
+        <v>-93.265011000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -843,8 +910,14 @@
       <c r="D11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>39.114052999999998</v>
+      </c>
+      <c r="F11">
+        <v>-94.627464000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -857,8 +930,14 @@
       <c r="D12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>40.712783999999999</v>
+      </c>
+      <c r="F12">
+        <v>-74.005941000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -871,8 +950,14 @@
       <c r="D13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>32.776663999999997</v>
+      </c>
+      <c r="F13">
+        <v>-96.796987999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -885,8 +970,14 @@
       <c r="D14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>35.467559999999999</v>
+      </c>
+      <c r="F14">
+        <v>-97.516428000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -899,8 +990,14 @@
       <c r="D15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>35.085334000000003</v>
+      </c>
+      <c r="F15">
+        <v>-106.605553</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -913,8 +1010,14 @@
       <c r="D16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>30.267153</v>
+      </c>
+      <c r="F16">
+        <v>-97.743060999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -927,8 +1030,14 @@
       <c r="D17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>33.448377000000001</v>
+      </c>
+      <c r="F17">
+        <v>-112.074037</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -941,8 +1050,14 @@
       <c r="D18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>36.169941000000001</v>
+      </c>
+      <c r="F18">
+        <v>-115.13983</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -955,8 +1070,14 @@
       <c r="D19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>34.052233999999999</v>
+      </c>
+      <c r="F19">
+        <v>-118.243685</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -969,8 +1090,14 @@
       <c r="D20" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>37.774929</v>
+      </c>
+      <c r="F20">
+        <v>-122.419416</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -983,8 +1110,14 @@
       <c r="D21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>45.523062000000003</v>
+      </c>
+      <c r="F21">
+        <v>-122.67648199999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -997,8 +1130,14 @@
       <c r="D22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>47.606209</v>
+      </c>
+      <c r="F22">
+        <v>-122.332071</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1011,8 +1150,14 @@
       <c r="D23" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>42.280825999999998</v>
+      </c>
+      <c r="F23">
+        <v>-83.743037999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1025,8 +1170,14 @@
       <c r="D24" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>39.952584000000002</v>
+      </c>
+      <c r="F24">
+        <v>-75.165222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1039,8 +1190,14 @@
       <c r="D25" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>41.823988999999997</v>
+      </c>
+      <c r="F25">
+        <v>-71.412834000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1053,8 +1210,14 @@
       <c r="D26" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>29.951066000000001</v>
+      </c>
+      <c r="F26">
+        <v>-90.071532000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1067,8 +1230,14 @@
       <c r="D27" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>25.761679999999998</v>
+      </c>
+      <c r="F27">
+        <v>-80.191789999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1081,8 +1250,14 @@
       <c r="D28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>29.424122000000001</v>
+      </c>
+      <c r="F28">
+        <v>-98.493628000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1095,8 +1270,14 @@
       <c r="D29" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>37.687176000000001</v>
+      </c>
+      <c r="F29">
+        <v>-97.330053000000007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1109,8 +1290,14 @@
       <c r="D30" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>39.768402999999999</v>
+      </c>
+      <c r="F30">
+        <v>-86.158068</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1122,6 +1309,12 @@
       </c>
       <c r="D31" t="s">
         <v>43</v>
+      </c>
+      <c r="E31">
+        <v>27.950575000000001</v>
+      </c>
+      <c r="F31">
+        <v>-82.457177999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>